<commit_message>
Sequencia de concepcao e imp. do sync - mapa de registros
</commit_message>
<xml_diff>
--- a/FPGA_Developments/Sync/sync_registers.xlsx
+++ b/FPGA_Developments/Sync/sync_registers.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11832"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="9372"/>
   </bookViews>
   <sheets>
     <sheet name="sync_regs" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">sync_regs!$B$2:$G$45</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">sync_regs!$B$2:$G$42</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="81">
   <si>
     <t>Register</t>
   </si>
@@ -62,45 +62,9 @@
     <t>Running status bit</t>
   </si>
   <si>
-    <t>Error status bit</t>
-  </si>
-  <si>
     <t>Internal/External_n status bit</t>
   </si>
   <si>
-    <t>Reseted interrupt enable bit</t>
-  </si>
-  <si>
-    <t>Reseted interrupt flag</t>
-  </si>
-  <si>
-    <t>Reseted interrupt flag clear</t>
-  </si>
-  <si>
-    <t>Channel A Output enable bit</t>
-  </si>
-  <si>
-    <t>Channel B Output enable bit</t>
-  </si>
-  <si>
-    <t>Channel C Output enable bit</t>
-  </si>
-  <si>
-    <t>Channel D Output enable bit</t>
-  </si>
-  <si>
-    <t>Channel E Output enable bit</t>
-  </si>
-  <si>
-    <t>Channel F Output enable bit</t>
-  </si>
-  <si>
-    <t>Channel G Output enable bit</t>
-  </si>
-  <si>
-    <t>Channel H Output enable bit</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -131,9 +95,6 @@
     <t>Signal polarity</t>
   </si>
   <si>
-    <t>Sync_out Output enable bit</t>
-  </si>
-  <si>
     <t>cycle number</t>
   </si>
   <si>
@@ -191,9 +152,6 @@
     <t>0 = idle / 1 = running</t>
   </si>
   <si>
-    <t>0 = no error / 1 = error</t>
-  </si>
-  <si>
     <t>0..255</t>
   </si>
   <si>
@@ -263,13 +221,55 @@
     <t>'0' allowed but is equivalent to '1'</t>
   </si>
   <si>
-    <t>Error Injection Emulation Register</t>
-  </si>
-  <si>
     <t>Obs: Register format: 32 bits:  &lt;31........0&gt; = Msb:Lsb</t>
   </si>
   <si>
     <t>Positive edge trigger</t>
+  </si>
+  <si>
+    <t>Sync Error Injection Register</t>
+  </si>
+  <si>
+    <t>Channel A output enable bit</t>
+  </si>
+  <si>
+    <t>Channel C output enable bit</t>
+  </si>
+  <si>
+    <t>Channel B output enable bit</t>
+  </si>
+  <si>
+    <t>Channel D output enable bit</t>
+  </si>
+  <si>
+    <t>Channel E output enable bit</t>
+  </si>
+  <si>
+    <t>Channel F output enable bit</t>
+  </si>
+  <si>
+    <t>Channel G output enable bit</t>
+  </si>
+  <si>
+    <t>Channel H output enable bit</t>
+  </si>
+  <si>
+    <t>Sync_out output enable bit</t>
+  </si>
+  <si>
+    <t>Error code</t>
+  </si>
+  <si>
+    <t>15:8</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>0..255 (codes: TBD)</t>
   </si>
 </sst>
 </file>
@@ -906,10 +906,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J46"/>
+  <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -926,7 +926,7 @@
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:10" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="B2" s="14" t="s">
         <v>0</v>
@@ -947,10 +947,10 @@
         <v>4</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="J2" s="36" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -958,7 +958,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="C3" s="17" t="s">
         <v>5</v>
@@ -974,7 +974,7 @@
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="3" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>10</v>
@@ -983,10 +983,10 @@
         <v>1</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -994,7 +994,7 @@
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="3" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>11</v>
@@ -1003,10 +1003,10 @@
         <v>1</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -1014,19 +1014,19 @@
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="3" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>12</v>
+        <v>76</v>
       </c>
       <c r="F6" s="2">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -1034,19 +1034,19 @@
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="3" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="F7" s="2">
         <v>8</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1064,7 +1064,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="C9" s="26" t="s">
         <v>5</v>
@@ -1080,10 +1080,10 @@
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="3" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="F10" s="2">
         <v>1</v>
@@ -1092,7 +1092,7 @@
         <v>6</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -1100,10 +1100,10 @@
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="F11" s="2">
         <v>1</v>
@@ -1112,7 +1112,7 @@
         <v>6</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -1120,10 +1120,10 @@
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="3" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="F12" s="2">
         <v>1</v>
@@ -1132,7 +1132,7 @@
         <v>6</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -1140,36 +1140,34 @@
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="3" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="F13" s="2">
         <v>1</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>57</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="H13" s="8"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="7"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="3" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="F14" s="2">
         <v>1</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H14" s="8"/>
     </row>
@@ -1178,52 +1176,52 @@
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="3" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="F15" s="2">
         <v>1</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H15" s="8"/>
+        <v>7</v>
+      </c>
+      <c r="H15" s="6"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="3" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="F16" s="2">
         <v>1</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H16" s="6"/>
+        <v>8</v>
+      </c>
+      <c r="H16" s="8"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="3" t="s">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="F17" s="2">
         <v>1</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H17" s="8"/>
     </row>
@@ -1232,309 +1230,315 @@
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="3" t="s">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="F18" s="2">
         <v>1</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H18" s="8"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="7"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F19" s="2">
-        <v>1</v>
-      </c>
-      <c r="G19" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H19" s="6"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="7"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F20" s="2">
-        <v>1</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H20" s="8"/>
+      <c r="H18" s="6"/>
+    </row>
+    <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="21"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="30"/>
+    </row>
+    <row r="20" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="31"/>
+      <c r="B20" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" s="28"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="29"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="7"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
+      <c r="A21" s="20">
+        <v>2</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>5</v>
+      </c>
       <c r="D21" s="3" t="s">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F21" s="2">
-        <v>1</v>
+        <v>17</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H21" s="8"/>
-    </row>
-    <row r="22" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="21"/>
-      <c r="B22" s="22"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="30"/>
-    </row>
-    <row r="23" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="31"/>
-      <c r="B23" s="26" t="s">
-        <v>72</v>
-      </c>
-      <c r="C23" s="28"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="29"/>
+        <v>6</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="20">
+        <v>3</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="20">
+        <v>4</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="20">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="C24" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H24" s="6" t="s">
-        <v>51</v>
-      </c>
+      <c r="D24" s="3"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="9"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="20">
-        <v>3</v>
-      </c>
-      <c r="B25" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="C25" s="19" t="s">
+      <c r="A25" s="20"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F25" s="2">
+        <v>1</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="20"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F26" s="2">
+        <v>8</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="32"/>
+      <c r="B27" s="33"/>
+      <c r="C27" s="33"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="34"/>
+    </row>
+    <row r="28" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="25">
+        <v>6</v>
+      </c>
+      <c r="B28" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H25" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="20">
-        <v>4</v>
-      </c>
-      <c r="B26" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="C26" s="19" t="s">
+      <c r="D28" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="F28" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="G28" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="H28" s="35" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="21"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="30"/>
+    </row>
+    <row r="30" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="25">
+        <v>7</v>
+      </c>
+      <c r="B30" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H26" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="20">
-        <v>5</v>
-      </c>
-      <c r="B27" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="C27" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="D27" s="3"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="9"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="20"/>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E28" s="2" t="s">
+      <c r="D30" s="27"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="28"/>
+      <c r="H30" s="29"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" s="7"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F31" s="2">
+        <v>1</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" s="7"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E32" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F28" s="2">
-        <v>1</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H28" s="9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="20"/>
-      <c r="B29" s="19"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F29" s="2">
-        <v>8</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H29" s="9" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="32"/>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="22"/>
-      <c r="G30" s="22"/>
-      <c r="H30" s="34"/>
-    </row>
-    <row r="31" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="25">
-        <v>6</v>
-      </c>
-      <c r="B31" s="26" t="s">
-        <v>78</v>
-      </c>
-      <c r="C31" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="D31" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="E31" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="F31" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="G31" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="H31" s="35" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="21"/>
-      <c r="B32" s="22"/>
-      <c r="C32" s="22"/>
-      <c r="D32" s="23"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="22"/>
-      <c r="G32" s="22"/>
-      <c r="H32" s="30"/>
-    </row>
-    <row r="33" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="25">
-        <v>7</v>
-      </c>
-      <c r="B33" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="C33" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="D33" s="27"/>
-      <c r="E33" s="28"/>
-      <c r="F33" s="28"/>
-      <c r="G33" s="28"/>
-      <c r="H33" s="29"/>
+      <c r="F32" s="2">
+        <v>1</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H32" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" s="7"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F33" s="2">
+        <v>1</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H33" s="6" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="7"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="3" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
       <c r="E34" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F34" s="2">
+        <v>1</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H34" s="6" t="s">
         <v>45</v>
-      </c>
-      <c r="F34" s="2">
-        <v>1</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H34" s="6" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
@@ -1542,10 +1546,10 @@
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="F35" s="2">
         <v>1</v>
@@ -1554,7 +1558,7 @@
         <v>6</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>80</v>
+        <v>45</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
@@ -1562,10 +1566,10 @@
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="3" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>47</v>
+        <v>68</v>
       </c>
       <c r="F36" s="2">
         <v>1</v>
@@ -1574,7 +1578,7 @@
         <v>6</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
@@ -1582,10 +1586,10 @@
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="3" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>16</v>
+        <v>70</v>
       </c>
       <c r="F37" s="2">
         <v>1</v>
@@ -1594,7 +1598,7 @@
         <v>6</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
@@ -1602,10 +1606,10 @@
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="3" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>17</v>
+        <v>71</v>
       </c>
       <c r="F38" s="2">
         <v>1</v>
@@ -1614,7 +1618,7 @@
         <v>6</v>
       </c>
       <c r="H38" s="6" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
@@ -1622,10 +1626,10 @@
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="3" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>18</v>
+        <v>72</v>
       </c>
       <c r="F39" s="2">
         <v>1</v>
@@ -1634,7 +1638,7 @@
         <v>6</v>
       </c>
       <c r="H39" s="6" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
@@ -1642,10 +1646,10 @@
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="3" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>19</v>
+        <v>73</v>
       </c>
       <c r="F40" s="2">
         <v>1</v>
@@ -1654,7 +1658,7 @@
         <v>6</v>
       </c>
       <c r="H40" s="6" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
@@ -1662,10 +1666,10 @@
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="3" t="s">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>20</v>
+        <v>74</v>
       </c>
       <c r="F41" s="2">
         <v>1</v>
@@ -1674,94 +1678,34 @@
         <v>6</v>
       </c>
       <c r="H41" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A42" s="7"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F42" s="2">
-        <v>1</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H42" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A43" s="7"/>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F43" s="2">
-        <v>1</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H43" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A44" s="7"/>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F44" s="2">
-        <v>1</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H44" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="10"/>
-      <c r="B45" s="11"/>
-      <c r="C45" s="11"/>
-      <c r="D45" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="E45" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="F45" s="11">
-        <v>1</v>
-      </c>
-      <c r="G45" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="H45" s="13" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="D46" s="1"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="10"/>
+      <c r="B42" s="11"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E42" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="F42" s="11">
+        <v>1</v>
+      </c>
+      <c r="G42" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H42" s="13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="D43" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="B2:G45"/>
+  <autoFilter ref="B2:G42"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Implementacao do modulo sync - update no mapa de registros
</commit_message>
<xml_diff>
--- a/FPGA_Developments/Sync/sync_registers.xlsx
+++ b/FPGA_Developments/Sync/sync_registers.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projetos\nsee\simucam_fpga\FPGA_Developments\Sync\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\cassio\repo_simucam\SimuCam_Development\FPGA_Developments\Sync\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="9372"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="9375"/>
   </bookViews>
   <sheets>
     <sheet name="sync_regs" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="93">
   <si>
     <t>Register</t>
   </si>
@@ -53,15 +53,9 @@
     <t>[R/-]</t>
   </si>
   <si>
-    <t>[-/W]</t>
-  </si>
-  <si>
     <t>Bit Field Position</t>
   </si>
   <si>
-    <t>Running status bit</t>
-  </si>
-  <si>
     <t>Internal/External_n status bit</t>
   </si>
   <si>
@@ -98,33 +92,12 @@
     <t>cycle number</t>
   </si>
   <si>
-    <t>Master Blank interrupt enable bit</t>
-  </si>
-  <si>
-    <t>Master Blank interrupt flag</t>
-  </si>
-  <si>
-    <t>Master Blank interrupt flag clear</t>
-  </si>
-  <si>
-    <t>Blank interrupt flag</t>
-  </si>
-  <si>
-    <t>Blank interrupt flag clear</t>
-  </si>
-  <si>
-    <t>Blank interrupt enable bit</t>
-  </si>
-  <si>
     <t>Error interrupt enable bit</t>
   </si>
   <si>
     <t>Error interrupt flag</t>
   </si>
   <si>
-    <t>Error interrupt flag clear</t>
-  </si>
-  <si>
     <t>Start</t>
   </si>
   <si>
@@ -143,15 +116,9 @@
     <t>Observação</t>
   </si>
   <si>
-    <t>clock base 50 MHz (@ 20 ns)</t>
-  </si>
-  <si>
     <t>Bits: TBD</t>
   </si>
   <si>
-    <t>0 = idle / 1 = running</t>
-  </si>
-  <si>
     <t>0..255</t>
   </si>
   <si>
@@ -161,9 +128,6 @@
     <t>0 = disable / 1 = enable</t>
   </si>
   <si>
-    <t>Level of blank pulses</t>
-  </si>
-  <si>
     <t>1 = enable</t>
   </si>
   <si>
@@ -176,9 +140,6 @@
     <t>9</t>
   </si>
   <si>
-    <t>10</t>
-  </si>
-  <si>
     <t>0 = ext sync / 1 = int sync</t>
   </si>
   <si>
@@ -200,9 +161,6 @@
     <t>7</t>
   </si>
   <si>
-    <t>11</t>
-  </si>
-  <si>
     <t>Sync Configuration Registers</t>
   </si>
   <si>
@@ -218,15 +176,9 @@
     <t>General</t>
   </si>
   <si>
-    <t>'0' allowed but is equivalent to '1'</t>
-  </si>
-  <si>
     <t>Obs: Register format: 32 bits:  &lt;31........0&gt; = Msb:Lsb</t>
   </si>
   <si>
-    <t>Positive edge trigger</t>
-  </si>
-  <si>
     <t>Sync Error Injection Register</t>
   </si>
   <si>
@@ -270,13 +222,97 @@
   </si>
   <si>
     <t>0..255 (codes: TBD)</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>0 = idle / 1 = running / 2 = one_shot / 3 = err_inj</t>
+  </si>
+  <si>
+    <t>Blank pulse interrupt enable bit</t>
+  </si>
+  <si>
+    <t>Blank pulse interrupt flag</t>
+  </si>
+  <si>
+    <t>7:2</t>
+  </si>
+  <si>
+    <t>Reserved</t>
+  </si>
+  <si>
+    <t>31:10</t>
+  </si>
+  <si>
+    <t>OST</t>
+  </si>
+  <si>
+    <t>One Shot time value</t>
+  </si>
+  <si>
+    <t>31:9</t>
+  </si>
+  <si>
+    <t>One_shot</t>
+  </si>
+  <si>
+    <t>Err_inj</t>
+  </si>
+  <si>
+    <t>Transition from idle to running state - positive edge trigger</t>
+  </si>
+  <si>
+    <t>Transition from running/error_inj to idle state - positive edge trigger</t>
+  </si>
+  <si>
+    <t>Transition from idle to error_inj state - positive edge trigger</t>
+  </si>
+  <si>
+    <t>23:16</t>
+  </si>
+  <si>
+    <t>30:24</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>30:20</t>
+  </si>
+  <si>
+    <t>15:9</t>
+  </si>
+  <si>
+    <t>Error conditions: TBD</t>
+  </si>
+  <si>
+    <t>Any blank pulses from any state</t>
+  </si>
+  <si>
+    <t>Transition from idle to one_shot state (automatic return) - positive edge trigger</t>
+  </si>
+  <si>
+    <t>It defines the level of blank pulses</t>
+  </si>
+  <si>
+    <t>Number of cycles of the "macro cycle". ''0' allowed but is equivalent to '1'</t>
+  </si>
+  <si>
+    <t>Base clock: 50 MHz (@ 20 ns)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -293,9 +329,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -534,7 +583,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -553,7 +602,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -564,9 +612,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -577,9 +622,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -625,7 +667,67 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -909,115 +1011,125 @@
   <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="33.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" customWidth="1"/>
-    <col min="4" max="4" width="20.88671875" customWidth="1"/>
-    <col min="5" max="5" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.88671875" customWidth="1"/>
-    <col min="7" max="7" width="10.88671875" customWidth="1"/>
+    <col min="2" max="2" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" customWidth="1"/>
+    <col min="5" max="5" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" customWidth="1"/>
     <col min="8" max="8" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:10" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" s="14" t="s">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:10" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="14" t="s">
+      <c r="C2" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="53" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="14">
+        <v>0</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="40" t="s">
+        <v>82</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="4" t="s">
+      <c r="F3" s="2">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="J2" s="36" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="16">
-        <v>0</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="18"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
-      <c r="D4" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="2">
-        <v>1</v>
-      </c>
-      <c r="G4" s="2" t="s">
+      <c r="D4" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="E4" s="41" t="s">
+        <v>70</v>
+      </c>
+      <c r="F4" s="41">
         <v>7</v>
       </c>
-      <c r="H4" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G4" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="42" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>11</v>
+        <v>65</v>
       </c>
       <c r="F5" s="2">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H5" s="33" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="3" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="F6" s="2">
         <v>8</v>
@@ -1026,18 +1138,18 @@
         <v>7</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="3" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F7" s="2">
         <v>8</v>
@@ -1046,44 +1158,54 @@
         <v>7</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="21"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="24"/>
-    </row>
-    <row r="9" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="25">
-        <v>1</v>
-      </c>
-      <c r="B9" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="18"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="21"/>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="22">
+        <v>1</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="27"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="29"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D9" s="43" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="F9" s="44">
+        <v>22</v>
+      </c>
+      <c r="G9" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="45" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="3" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="F10" s="2">
         <v>1</v>
@@ -1092,18 +1214,18 @@
         <v>6</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="3" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>23</v>
+        <v>67</v>
       </c>
       <c r="F11" s="2">
         <v>1</v>
@@ -1112,364 +1234,402 @@
         <v>6</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
-      <c r="D12" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" s="2">
-        <v>1</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D12" s="39" t="s">
+        <v>69</v>
+      </c>
+      <c r="E12" s="41" t="s">
+        <v>70</v>
+      </c>
+      <c r="F12" s="41">
+        <v>6</v>
+      </c>
+      <c r="G12" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="46" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="3" t="s">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="F13" s="2">
         <v>1</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H13" s="8"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="H13" s="34" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="3" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="E14" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F14" s="2">
+        <v>1</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H14" s="34" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="18"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="27"/>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="28"/>
+      <c r="B16" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="25"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="26"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="17">
+        <v>2</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="17">
+        <v>3</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="17">
+        <v>4</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="17">
+        <v>5</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="17">
+        <v>6</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="39" t="s">
+        <v>74</v>
+      </c>
+      <c r="E21" s="41" t="s">
+        <v>70</v>
+      </c>
+      <c r="F21" s="41">
+        <v>23</v>
+      </c>
+      <c r="G21" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="H21" s="47" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="17"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F22" s="2">
+        <v>1</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="17"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F14" s="2">
-        <v>1</v>
-      </c>
-      <c r="G14" s="2" t="s">
+      <c r="E23" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" s="2">
         <v>8</v>
       </c>
-      <c r="H14" s="8"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="7"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F15" s="2">
-        <v>1</v>
-      </c>
-      <c r="G15" s="2" t="s">
+      <c r="G23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H23" s="52" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="29"/>
+      <c r="B24" s="30"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="31"/>
+    </row>
+    <row r="25" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="22">
         <v>7</v>
       </c>
-      <c r="H15" s="6"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="7"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F16" s="2">
-        <v>1</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H16" s="8"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="7"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F17" s="2">
-        <v>1</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H17" s="8"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="7"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F18" s="2">
-        <v>1</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H18" s="6"/>
-    </row>
-    <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="21"/>
-      <c r="B19" s="22"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="30"/>
-    </row>
-    <row r="20" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="31"/>
-      <c r="B20" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="C20" s="28"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="29"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="20">
-        <v>2</v>
-      </c>
-      <c r="B21" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="C21" s="19" t="s">
+      <c r="B25" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H21" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="20">
-        <v>3</v>
-      </c>
-      <c r="B22" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="C22" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H22" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="20">
-        <v>4</v>
-      </c>
-      <c r="B23" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="C23" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H23" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="20">
-        <v>5</v>
-      </c>
-      <c r="B24" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="C24" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24" s="3"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="9"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="20"/>
-      <c r="B25" s="19"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F25" s="2">
-        <v>1</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H25" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="20"/>
+      <c r="D25" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="G25" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="H25" s="32" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="18"/>
       <c r="B26" s="19"/>
       <c r="C26" s="19"/>
-      <c r="D26" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F26" s="2">
+      <c r="D26" s="20"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="27"/>
+    </row>
+    <row r="27" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="22">
         <v>8</v>
       </c>
-      <c r="G26" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H26" s="9" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="32"/>
-      <c r="B27" s="33"/>
-      <c r="C27" s="33"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="34"/>
-    </row>
-    <row r="28" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="25">
-        <v>6</v>
-      </c>
-      <c r="B28" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="C28" s="26" t="s">
+      <c r="B27" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D28" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="E28" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="F28" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="G28" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="H28" s="35" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="21"/>
-      <c r="B29" s="22"/>
-      <c r="C29" s="22"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="22"/>
-      <c r="G29" s="22"/>
-      <c r="H29" s="30"/>
-    </row>
-    <row r="30" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="25">
-        <v>7</v>
-      </c>
-      <c r="B30" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="C30" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="D30" s="27"/>
-      <c r="E30" s="28"/>
-      <c r="F30" s="28"/>
-      <c r="G30" s="28"/>
-      <c r="H30" s="29"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D27" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="E27" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="F27" s="25">
+        <v>1</v>
+      </c>
+      <c r="G27" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="H27" s="36" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="37"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="48" t="s">
+        <v>85</v>
+      </c>
+      <c r="E28" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="F28" s="49">
+        <v>11</v>
+      </c>
+      <c r="G28" s="49" t="s">
+        <v>10</v>
+      </c>
+      <c r="H28" s="50" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="7"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F29" s="2">
+        <v>1</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H29" s="33" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="7"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F30" s="2">
+        <v>1</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H30" s="33" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="3" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>32</v>
+        <v>75</v>
       </c>
       <c r="F31" s="2">
         <v>1</v>
@@ -1477,19 +1637,19 @@
       <c r="G31" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H31" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H31" s="33" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="3" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
       <c r="F32" s="2">
         <v>1</v>
@@ -1497,39 +1657,39 @@
       <c r="G32" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H32" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H32" s="33" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
-      <c r="D33" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F33" s="2">
-        <v>1</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H33" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D33" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="E33" s="41" t="s">
+        <v>70</v>
+      </c>
+      <c r="F33" s="41">
+        <v>7</v>
+      </c>
+      <c r="G33" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="H33" s="51" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="3" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="F34" s="2">
         <v>1</v>
@@ -1537,19 +1697,19 @@
       <c r="G34" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H34" s="6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H34" s="33" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="3" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="F35" s="2">
         <v>1</v>
@@ -1557,19 +1717,19 @@
       <c r="G35" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H35" s="6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H35" s="33" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="3" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="F36" s="2">
         <v>1</v>
@@ -1577,19 +1737,19 @@
       <c r="G36" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H36" s="6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H36" s="33" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="3" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="F37" s="2">
         <v>1</v>
@@ -1597,19 +1757,19 @@
       <c r="G37" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H37" s="6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H37" s="33" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="3" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="F38" s="2">
         <v>1</v>
@@ -1617,19 +1777,19 @@
       <c r="G38" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H38" s="6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H38" s="33" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="3" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="F39" s="2">
         <v>1</v>
@@ -1637,19 +1797,19 @@
       <c r="G39" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H39" s="6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H39" s="33" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="3" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="F40" s="2">
         <v>1</v>
@@ -1657,19 +1817,19 @@
       <c r="G40" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H40" s="6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H40" s="33" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="3" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="F41" s="2">
         <v>1</v>
@@ -1677,31 +1837,31 @@
       <c r="G41" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H41" s="6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="10"/>
-      <c r="B42" s="11"/>
-      <c r="C42" s="11"/>
-      <c r="D42" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="E42" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="F42" s="11">
-        <v>1</v>
-      </c>
-      <c r="G42" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="H42" s="13" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="H41" s="33" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="9"/>
+      <c r="B42" s="10"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F42" s="10">
+        <v>1</v>
+      </c>
+      <c r="G42" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H42" s="35" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D43" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Novo conceito: interrupcoes gerenciadas por componente int. Mapa de registros alterado, e inicio das adaptacoes nos fontes vhdl
</commit_message>
<xml_diff>
--- a/FPGA_Developments/Sync/sync_registers.xlsx
+++ b/FPGA_Developments/Sync/sync_registers.xlsx
@@ -15,7 +15,7 @@
     <sheet name="sync_regs" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">sync_regs!$B$2:$G$42</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">sync_regs!$B$2:$G$48</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="97">
   <si>
     <t>Register</t>
   </si>
@@ -68,9 +68,6 @@
     <t>Sync Control Register</t>
   </si>
   <si>
-    <t>Sync Interrupt Register</t>
-  </si>
-  <si>
     <t>Error injection emulation</t>
   </si>
   <si>
@@ -137,9 +134,6 @@
     <t>8</t>
   </si>
   <si>
-    <t>9</t>
-  </si>
-  <si>
     <t>0 = ext sync / 1 = int sync</t>
   </si>
   <si>
@@ -236,15 +230,9 @@
     <t>Blank pulse interrupt flag</t>
   </si>
   <si>
-    <t>7:2</t>
-  </si>
-  <si>
     <t>Reserved</t>
   </si>
   <si>
-    <t>31:10</t>
-  </si>
-  <si>
     <t>OST</t>
   </si>
   <si>
@@ -306,6 +294,30 @@
   </si>
   <si>
     <t>Base clock: 50 MHz (@ 20 ns)</t>
+  </si>
+  <si>
+    <t>Sync Interrupt Registers</t>
+  </si>
+  <si>
+    <t>Enable</t>
+  </si>
+  <si>
+    <t>Flag</t>
+  </si>
+  <si>
+    <t>31:2</t>
+  </si>
+  <si>
+    <t>Error interrupt flag clear</t>
+  </si>
+  <si>
+    <t>Blank pulse interrupt flag clear</t>
+  </si>
+  <si>
+    <t>"1" to clear int flag</t>
+  </si>
+  <si>
+    <t>Flag clear</t>
   </si>
 </sst>
 </file>
@@ -358,7 +370,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -579,11 +591,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -697,15 +748,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -728,6 +770,20 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1008,10 +1064,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J43"/>
+  <dimension ref="A1:J49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1028,7 +1084,7 @@
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:10" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>0</v>
@@ -1049,10 +1105,10 @@
         <v>4</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J2" s="53" t="s">
-        <v>49</v>
+        <v>27</v>
+      </c>
+      <c r="J2" s="50" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1066,7 +1122,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="40" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>9</v>
@@ -1078,7 +1134,7 @@
         <v>7</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1086,10 +1142,10 @@
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="39" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E4" s="41" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F4" s="41">
         <v>7</v>
@@ -1106,10 +1162,10 @@
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F5" s="2">
         <v>8</v>
@@ -1118,7 +1174,7 @@
         <v>7</v>
       </c>
       <c r="H5" s="33" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1126,10 +1182,10 @@
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F6" s="2">
         <v>8</v>
@@ -1138,7 +1194,7 @@
         <v>7</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1146,10 +1202,10 @@
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F7" s="2">
         <v>8</v>
@@ -1158,7 +1214,7 @@
         <v>7</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1172,49 +1228,41 @@
       <c r="H8" s="21"/>
     </row>
     <row r="9" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="22">
-        <v>1</v>
-      </c>
-      <c r="B9" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="23" t="s">
+      <c r="A9" s="51"/>
+      <c r="B9" s="52" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9" s="53"/>
+      <c r="D9" s="54"/>
+      <c r="E9" s="53"/>
+      <c r="F9" s="53"/>
+      <c r="G9" s="53"/>
+      <c r="H9" s="55"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="17">
+        <v>1</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="43" t="s">
-        <v>71</v>
-      </c>
-      <c r="E9" s="44" t="s">
-        <v>70</v>
-      </c>
-      <c r="F9" s="44">
-        <v>22</v>
-      </c>
-      <c r="G9" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="H9" s="45" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10" s="2">
-        <v>1</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>32</v>
+      <c r="D10" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="E10" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="F10" s="41">
+        <v>30</v>
+      </c>
+      <c r="G10" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="43" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1222,10 +1270,10 @@
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="3" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>67</v>
+        <v>20</v>
       </c>
       <c r="F11" s="2">
         <v>1</v>
@@ -1234,482 +1282,474 @@
         <v>6</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
-      <c r="D12" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="E12" s="41" t="s">
-        <v>70</v>
-      </c>
-      <c r="F12" s="41">
-        <v>6</v>
-      </c>
-      <c r="G12" s="41" t="s">
-        <v>10</v>
-      </c>
-      <c r="H12" s="46" t="s">
-        <v>10</v>
+      <c r="D12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" s="2">
-        <v>1</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H13" s="34" t="s">
-        <v>87</v>
-      </c>
+      <c r="A13" s="17"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="6"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="3" t="s">
+      <c r="A14" s="17">
+        <v>2</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="E14" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="F14" s="41">
+        <v>30</v>
+      </c>
+      <c r="G14" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="43" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F14" s="2">
-        <v>1</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H14" s="34" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="18"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="27"/>
-    </row>
-    <row r="16" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="28"/>
-      <c r="B16" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" s="25"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="26"/>
+      <c r="E15" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F15" s="2">
+        <v>1</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H15" s="56" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="7"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F16" s="2">
+        <v>1</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H16" s="56" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="17">
-        <v>2</v>
-      </c>
-      <c r="B17" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H17" s="6" t="s">
-        <v>92</v>
-      </c>
+      <c r="A17" s="17"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="6"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="17">
         <v>3</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>46</v>
+        <v>91</v>
       </c>
       <c r="C18" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18" s="2" t="s">
+      <c r="D18" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="E18" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="F18" s="41">
+        <v>30</v>
+      </c>
+      <c r="G18" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" s="43" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="7"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" s="2">
+        <v>1</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H19" s="34" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="7"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F20" s="2">
+        <v>1</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H20" s="34" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="18"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="27"/>
+    </row>
+    <row r="22" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="28"/>
+      <c r="B22" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="25"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="26"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="17">
+        <v>4</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="17">
+        <v>5</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="17">
+        <v>6</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F18" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H18" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="17">
-        <v>4</v>
-      </c>
-      <c r="B19" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="C19" s="16" t="s">
+      <c r="F25" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="17">
+        <v>7</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C26" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19" s="2" t="s">
+      <c r="D26" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="17">
+        <v>8</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" s="39" t="s">
+        <v>70</v>
+      </c>
+      <c r="E27" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="F27" s="41">
+        <v>23</v>
+      </c>
+      <c r="G27" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="H27" s="44" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="17"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F28" s="2">
+        <v>1</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H28" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="17"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E29" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F19" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="17">
+      <c r="F29" s="2">
+        <v>8</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H29" s="49" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="29"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="31"/>
+    </row>
+    <row r="31" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="22">
+        <v>9</v>
+      </c>
+      <c r="B31" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="C31" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="C20" s="16" t="s">
+      <c r="D31" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="F31" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="G31" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="H31" s="32" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="18"/>
+      <c r="B32" s="19"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="27"/>
+    </row>
+    <row r="33" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="22">
+        <v>10</v>
+      </c>
+      <c r="B33" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="17">
-        <v>6</v>
-      </c>
-      <c r="B21" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" s="39" t="s">
-        <v>74</v>
-      </c>
-      <c r="E21" s="41" t="s">
-        <v>70</v>
-      </c>
-      <c r="F21" s="41">
-        <v>23</v>
-      </c>
-      <c r="G21" s="41" t="s">
-        <v>10</v>
-      </c>
-      <c r="H21" s="47" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="17"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="3" t="s">
+      <c r="D33" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="E33" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="F33" s="25">
+        <v>1</v>
+      </c>
+      <c r="G33" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="H33" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="E22" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F22" s="2">
-        <v>1</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H22" s="8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="17"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F23" s="2">
-        <v>8</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H23" s="52" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="29"/>
-      <c r="B24" s="30"/>
-      <c r="C24" s="30"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="31"/>
-    </row>
-    <row r="25" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="22">
-        <v>7</v>
-      </c>
-      <c r="B25" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="C25" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="D25" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="E25" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="F25" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="G25" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="H25" s="32" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="18"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="27"/>
-    </row>
-    <row r="27" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="22">
-        <v>8</v>
-      </c>
-      <c r="B27" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="C27" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="D27" s="24" t="s">
-        <v>82</v>
-      </c>
-      <c r="E27" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="F27" s="25">
-        <v>1</v>
-      </c>
-      <c r="G27" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="H27" s="36" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="37"/>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="48" t="s">
-        <v>85</v>
-      </c>
-      <c r="E28" s="49" t="s">
-        <v>70</v>
-      </c>
-      <c r="F28" s="49">
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="37"/>
+      <c r="B34" s="38"/>
+      <c r="C34" s="38"/>
+      <c r="D34" s="45" t="s">
+        <v>81</v>
+      </c>
+      <c r="E34" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="F34" s="46">
         <v>11</v>
       </c>
-      <c r="G28" s="49" t="s">
-        <v>10</v>
-      </c>
-      <c r="H28" s="50" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F29" s="2">
-        <v>1</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H29" s="33" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="7"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F30" s="2">
-        <v>1</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H30" s="33" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F31" s="2">
-        <v>1</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H31" s="33" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="7"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F32" s="2">
-        <v>1</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H32" s="33" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="7"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="39" t="s">
-        <v>86</v>
-      </c>
-      <c r="E33" s="41" t="s">
-        <v>70</v>
-      </c>
-      <c r="F33" s="41">
-        <v>7</v>
-      </c>
-      <c r="G33" s="41" t="s">
-        <v>10</v>
-      </c>
-      <c r="H33" s="51" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="7"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F34" s="2">
-        <v>1</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H34" s="33" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G34" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="H34" s="47" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="3" t="s">
-        <v>43</v>
+        <v>80</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>58</v>
+        <v>22</v>
       </c>
       <c r="F35" s="2">
         <v>1</v>
@@ -1718,18 +1758,18 @@
         <v>6</v>
       </c>
       <c r="H35" s="33" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="3" t="s">
-        <v>42</v>
+        <v>79</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>57</v>
+        <v>23</v>
       </c>
       <c r="F36" s="2">
         <v>1</v>
@@ -1738,18 +1778,18 @@
         <v>6</v>
       </c>
       <c r="H36" s="33" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="3" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="F37" s="2">
         <v>1</v>
@@ -1758,18 +1798,18 @@
         <v>6</v>
       </c>
       <c r="H37" s="33" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="3" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="F38" s="2">
         <v>1</v>
@@ -1778,27 +1818,27 @@
         <v>6</v>
       </c>
       <c r="H38" s="33" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
-      <c r="D39" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F39" s="2">
-        <v>1</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H39" s="33" t="s">
-        <v>33</v>
+      <c r="D39" s="39" t="s">
+        <v>82</v>
+      </c>
+      <c r="E39" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="F39" s="41">
+        <v>7</v>
+      </c>
+      <c r="G39" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="H39" s="48" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -1806,10 +1846,10 @@
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="F40" s="2">
         <v>1</v>
@@ -1818,7 +1858,7 @@
         <v>6</v>
       </c>
       <c r="H40" s="33" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -1826,46 +1866,166 @@
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="3" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="E41" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F41" s="2">
+        <v>1</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H41" s="33" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="7"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F42" s="2">
+        <v>1</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H42" s="33" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="7"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F43" s="2">
+        <v>1</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H43" s="33" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="7"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E44" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F41" s="2">
-        <v>1</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H41" s="33" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="9"/>
-      <c r="B42" s="10"/>
-      <c r="C42" s="10"/>
-      <c r="D42" s="11" t="s">
+      <c r="F44" s="2">
+        <v>1</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H44" s="33" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="7"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F45" s="2">
+        <v>1</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H45" s="33" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="7"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F46" s="2">
+        <v>1</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H46" s="33" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="7"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E42" s="10" t="s">
+      <c r="E47" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F42" s="10">
-        <v>1</v>
-      </c>
-      <c r="G42" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="H42" s="35" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="D43" s="1"/>
+      <c r="F47" s="2">
+        <v>1</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H47" s="33" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="9"/>
+      <c r="B48" s="10"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E48" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="F48" s="10">
+        <v>1</v>
+      </c>
+      <c r="G48" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H48" s="35" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="49" spans="4:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D49" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="B2:G42"/>
+  <autoFilter ref="B2:G48"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Validacao do modulo sync em modelsim
</commit_message>
<xml_diff>
--- a/FPGA_Developments/Sync/sync_registers.xlsx
+++ b/FPGA_Developments/Sync/sync_registers.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\cassio\repo_simucam\SimuCam_Development\FPGA_Developments\Sync\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projetos\nsee\simucam_fpga\FPGA_Developments\Sync\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="9375"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="9372"/>
   </bookViews>
   <sheets>
     <sheet name="sync_regs" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="98">
   <si>
     <t>Register</t>
   </si>
@@ -318,6 +318,9 @@
   </si>
   <si>
     <t>Flag clear</t>
+  </si>
+  <si>
+    <t>Reset Value</t>
   </si>
 </sst>
 </file>
@@ -370,7 +373,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -630,11 +633,83 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -783,6 +858,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1064,25 +1160,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J49"/>
+  <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="H50" sqref="H50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" customWidth="1"/>
-    <col min="5" max="5" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" customWidth="1"/>
-    <col min="8" max="8" width="32" customWidth="1"/>
+    <col min="2" max="2" width="25.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.88671875" customWidth="1"/>
+    <col min="5" max="5" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="57.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:10" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:11" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>33</v>
       </c>
@@ -1104,14 +1201,17 @@
       <c r="G2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="J2" s="50" t="s">
+      <c r="K2" s="50" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="14">
         <v>0</v>
       </c>
@@ -1133,11 +1233,14 @@
       <c r="G3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="57">
+        <v>0</v>
+      </c>
+      <c r="I3" s="6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -1153,11 +1256,14 @@
       <c r="G4" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="42" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="H4" s="58" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="42" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -1173,11 +1279,14 @@
       <c r="G5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="33" t="s">
+      <c r="H5" s="57">
+        <v>0</v>
+      </c>
+      <c r="I5" s="33" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -1193,11 +1302,14 @@
       <c r="G6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="57">
+        <v>0</v>
+      </c>
+      <c r="I6" s="6" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -1213,11 +1325,14 @@
       <c r="G7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="57">
+        <v>0</v>
+      </c>
+      <c r="I7" s="6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="18"/>
       <c r="B8" s="19"/>
       <c r="C8" s="19"/>
@@ -1225,9 +1340,10 @@
       <c r="E8" s="19"/>
       <c r="F8" s="19"/>
       <c r="G8" s="19"/>
-      <c r="H8" s="21"/>
-    </row>
-    <row r="9" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="H8" s="59"/>
+      <c r="I8" s="21"/>
+    </row>
+    <row r="9" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A9" s="51"/>
       <c r="B9" s="52" t="s">
         <v>89</v>
@@ -1237,9 +1353,10 @@
       <c r="E9" s="53"/>
       <c r="F9" s="53"/>
       <c r="G9" s="53"/>
-      <c r="H9" s="55"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H9" s="60"/>
+      <c r="I9" s="55"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="17">
         <v>1</v>
       </c>
@@ -1261,11 +1378,12 @@
       <c r="G10" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="43" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H10" s="58"/>
+      <c r="I10" s="43" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="7"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -1281,11 +1399,14 @@
       <c r="G11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="57">
+        <v>0</v>
+      </c>
+      <c r="I11" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="7"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -1301,11 +1422,14 @@
       <c r="G12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="H12" s="57">
+        <v>0</v>
+      </c>
+      <c r="I12" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="17"/>
       <c r="B13" s="16"/>
       <c r="C13" s="16"/>
@@ -1313,9 +1437,10 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
-      <c r="H13" s="6"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H13" s="57"/>
+      <c r="I13" s="6"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="17">
         <v>2</v>
       </c>
@@ -1337,11 +1462,12 @@
       <c r="G14" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="H14" s="43" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H14" s="58"/>
+      <c r="I14" s="43" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -1357,11 +1483,14 @@
       <c r="G15" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H15" s="56" t="s">
+      <c r="H15" s="57">
+        <v>0</v>
+      </c>
+      <c r="I15" s="56" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -1377,11 +1506,14 @@
       <c r="G16" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H16" s="56" t="s">
+      <c r="H16" s="57">
+        <v>0</v>
+      </c>
+      <c r="I16" s="56" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="17"/>
       <c r="B17" s="16"/>
       <c r="C17" s="16"/>
@@ -1389,9 +1521,10 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
-      <c r="H17" s="6"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H17" s="57"/>
+      <c r="I17" s="6"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="17">
         <v>3</v>
       </c>
@@ -1413,11 +1546,12 @@
       <c r="G18" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="H18" s="43" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H18" s="58"/>
+      <c r="I18" s="43" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -1433,11 +1567,14 @@
       <c r="G19" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H19" s="34" t="s">
+      <c r="H19" s="57">
+        <v>0</v>
+      </c>
+      <c r="I19" s="34" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -1453,11 +1590,14 @@
       <c r="G20" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H20" s="34" t="s">
+      <c r="H20" s="57">
+        <v>0</v>
+      </c>
+      <c r="I20" s="34" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="18"/>
       <c r="B21" s="19"/>
       <c r="C21" s="19"/>
@@ -1465,9 +1605,10 @@
       <c r="E21" s="19"/>
       <c r="F21" s="19"/>
       <c r="G21" s="19"/>
-      <c r="H21" s="27"/>
-    </row>
-    <row r="22" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="H21" s="59"/>
+      <c r="I21" s="27"/>
+    </row>
+    <row r="22" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A22" s="28"/>
       <c r="B22" s="23" t="s">
         <v>42</v>
@@ -1477,9 +1618,10 @@
       <c r="E22" s="25"/>
       <c r="F22" s="25"/>
       <c r="G22" s="25"/>
-      <c r="H22" s="26"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H22" s="61"/>
+      <c r="I22" s="26"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="17">
         <v>4</v>
       </c>
@@ -1501,11 +1643,14 @@
       <c r="G23" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H23" s="6" t="s">
+      <c r="H23" s="57">
+        <v>0</v>
+      </c>
+      <c r="I23" s="6" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="17">
         <v>5</v>
       </c>
@@ -1527,11 +1672,14 @@
       <c r="G24" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H24" s="6" t="s">
+      <c r="H24" s="57">
+        <v>0</v>
+      </c>
+      <c r="I24" s="6" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="17">
         <v>6</v>
       </c>
@@ -1553,11 +1701,14 @@
       <c r="G25" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H25" s="6" t="s">
+      <c r="H25" s="57">
+        <v>0</v>
+      </c>
+      <c r="I25" s="6" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="17">
         <v>7</v>
       </c>
@@ -1579,11 +1730,14 @@
       <c r="G26" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H26" s="6" t="s">
+      <c r="H26" s="57">
+        <v>0</v>
+      </c>
+      <c r="I26" s="6" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="17">
         <v>8</v>
       </c>
@@ -1605,11 +1759,14 @@
       <c r="G27" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="H27" s="44" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H27" s="58" t="s">
+        <v>10</v>
+      </c>
+      <c r="I27" s="44" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="17"/>
       <c r="B28" s="16"/>
       <c r="C28" s="16"/>
@@ -1625,11 +1782,14 @@
       <c r="G28" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H28" s="8" t="s">
+      <c r="H28" s="57">
+        <v>0</v>
+      </c>
+      <c r="I28" s="8" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="17"/>
       <c r="B29" s="16"/>
       <c r="C29" s="16"/>
@@ -1645,11 +1805,14 @@
       <c r="G29" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H29" s="49" t="s">
+      <c r="H29" s="57">
+        <v>0</v>
+      </c>
+      <c r="I29" s="49" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="29"/>
       <c r="B30" s="30"/>
       <c r="C30" s="30"/>
@@ -1657,9 +1820,10 @@
       <c r="E30" s="19"/>
       <c r="F30" s="19"/>
       <c r="G30" s="19"/>
-      <c r="H30" s="31"/>
-    </row>
-    <row r="31" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="H30" s="59"/>
+      <c r="I30" s="31"/>
+    </row>
+    <row r="31" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A31" s="22">
         <v>9</v>
       </c>
@@ -1681,11 +1845,14 @@
       <c r="G31" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="H31" s="32" t="s">
+      <c r="H31" s="61">
+        <v>0</v>
+      </c>
+      <c r="I31" s="32" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="18"/>
       <c r="B32" s="19"/>
       <c r="C32" s="19"/>
@@ -1693,9 +1860,10 @@
       <c r="E32" s="19"/>
       <c r="F32" s="19"/>
       <c r="G32" s="19"/>
-      <c r="H32" s="27"/>
-    </row>
-    <row r="33" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="H32" s="59"/>
+      <c r="I32" s="27"/>
+    </row>
+    <row r="33" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A33" s="22">
         <v>10</v>
       </c>
@@ -1717,11 +1885,14 @@
       <c r="G33" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="H33" s="36" t="s">
+      <c r="H33" s="61">
+        <v>0</v>
+      </c>
+      <c r="I33" s="36" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="37"/>
       <c r="B34" s="38"/>
       <c r="C34" s="38"/>
@@ -1737,11 +1908,14 @@
       <c r="G34" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="H34" s="47" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="H34" s="62" t="s">
+        <v>10</v>
+      </c>
+      <c r="I34" s="47" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="7"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -1757,11 +1931,14 @@
       <c r="G35" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H35" s="33" t="s">
+      <c r="H35" s="57">
+        <v>0</v>
+      </c>
+      <c r="I35" s="33" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="7"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -1777,11 +1954,14 @@
       <c r="G36" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H36" s="33" t="s">
+      <c r="H36" s="57">
+        <v>0</v>
+      </c>
+      <c r="I36" s="33" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="7"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -1797,11 +1977,14 @@
       <c r="G37" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H37" s="33" t="s">
+      <c r="H37" s="57">
+        <v>0</v>
+      </c>
+      <c r="I37" s="33" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="7"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -1817,11 +2000,14 @@
       <c r="G38" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H38" s="33" t="s">
+      <c r="H38" s="57">
+        <v>0</v>
+      </c>
+      <c r="I38" s="33" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="7"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -1837,11 +2023,14 @@
       <c r="G39" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="H39" s="48" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H39" s="58" t="s">
+        <v>10</v>
+      </c>
+      <c r="I39" s="48" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="7"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -1857,11 +2046,14 @@
       <c r="G40" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H40" s="33" t="s">
+      <c r="H40" s="57">
+        <v>0</v>
+      </c>
+      <c r="I40" s="33" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="7"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -1877,11 +2069,14 @@
       <c r="G41" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H41" s="33" t="s">
+      <c r="H41" s="57">
+        <v>0</v>
+      </c>
+      <c r="I41" s="33" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="7"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -1897,11 +2092,14 @@
       <c r="G42" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H42" s="33" t="s">
+      <c r="H42" s="57">
+        <v>0</v>
+      </c>
+      <c r="I42" s="33" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="7"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -1917,11 +2115,14 @@
       <c r="G43" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H43" s="33" t="s">
+      <c r="H43" s="57">
+        <v>0</v>
+      </c>
+      <c r="I43" s="33" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="7"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -1937,11 +2138,14 @@
       <c r="G44" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H44" s="33" t="s">
+      <c r="H44" s="57">
+        <v>0</v>
+      </c>
+      <c r="I44" s="33" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="7"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -1957,11 +2161,14 @@
       <c r="G45" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H45" s="33" t="s">
+      <c r="H45" s="57">
+        <v>0</v>
+      </c>
+      <c r="I45" s="33" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="7"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -1977,11 +2184,14 @@
       <c r="G46" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H46" s="33" t="s">
+      <c r="H46" s="57">
+        <v>0</v>
+      </c>
+      <c r="I46" s="33" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="7"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -1997,11 +2207,14 @@
       <c r="G47" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H47" s="33" t="s">
+      <c r="H47" s="57">
+        <v>0</v>
+      </c>
+      <c r="I47" s="33" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="9"/>
       <c r="B48" s="10"/>
       <c r="C48" s="10"/>
@@ -2017,11 +2230,14 @@
       <c r="G48" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H48" s="35" t="s">
+      <c r="H48" s="63">
+        <v>0</v>
+      </c>
+      <c r="I48" s="35" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="49" spans="4:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="D49" s="1"/>
     </row>
   </sheetData>

</xml_diff>